<commit_message>
Fix OPF cases and dynamic cases
</commit_message>
<xml_diff>
--- a/ACTIVSg200/IL200_dyn.xlsx
+++ b/ACTIVSg200/IL200_dyn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/turbinegov/ACTIVSg200/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F352BA-93BA-514F-937E-8F18D6257407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A532AD2-CE99-5C4C-B7CB-67CFA399970A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -19192,9 +19192,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20106,7 +20106,7 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>16</v>
@@ -20162,7 +20162,7 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -20330,7 +20330,7 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>20</v>
@@ -21282,7 +21282,7 @@
         <v>37</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <v>37</v>
@@ -21338,7 +21338,7 @@
         <v>38</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <v>38</v>
@@ -21394,7 +21394,7 @@
         <v>39</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>39</v>
@@ -21450,7 +21450,7 @@
         <v>40</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41">
         <v>40</v>
@@ -21562,7 +21562,7 @@
         <v>42</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43">
         <v>42</v>
@@ -21618,7 +21618,7 @@
         <v>43</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44">
         <v>43</v>
@@ -21842,7 +21842,7 @@
         <v>48</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48">
         <v>48</v>
@@ -21898,7 +21898,7 @@
         <v>49</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
         <v>49</v>
@@ -40542,8 +40542,8 @@
   <dimension ref="A1:AE50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" activeCellId="3" sqref="E38 E40 E49 E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -45013,7 +45013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P30" sqref="P30"/>
     </sheetView>

</xml_diff>